<commit_message>
Examples Analysis and Conversion Utilities
- Introduced analyzeExamples.m and convertExamples.m for batch analysis and conversion of data model files in the Examples directory.
- Enhanced cType and cMessages with new options and messages for model formats and batch operations.
- Added filesInfo.m function  for recursive file discovery.
- Improve cReadModel,  to better support of TaesLabPath features.
- Removed obsolete and duplicate example files, and updated documentation and function comments accordingly.
</commit_message>
<xml_diff>
--- a/Examples/scgp/scgp0_model.xlsx
+++ b/Examples/scgp/scgp0_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Termoeconomia\ExIOLab\Examples\kotas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\scgp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2830FB04-2DF4-4DBF-B93E-831D937EA115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF7922B-E76C-4053-A3E2-8797CACCCD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="6" r:id="rId1"/>
@@ -516,9 +516,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -556,7 +556,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -662,7 +662,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -804,7 +804,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1084,15 +1084,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1100,7 +1101,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -1109,7 +1110,7 @@
         <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1117,7 +1118,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1126,7 +1127,7 @@
         <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1134,7 +1135,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1143,7 +1144,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1151,7 +1152,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -1160,7 +1161,7 @@
         <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1168,7 +1169,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -1177,7 +1178,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1185,7 +1186,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -1194,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1202,7 +1203,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -1211,7 +1212,7 @@
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1219,7 +1220,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -1228,7 +1229,7 @@
         <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1236,7 +1237,7 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
@@ -1245,7 +1246,7 @@
         <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1253,7 +1254,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -1262,7 +1263,7 @@
         <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89C2992-CD54-4B22-B5B6-C9FA79546F3C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>